<commit_message>
TS implemented using different strategies.
</commit_message>
<xml_diff>
--- a/TS_HW5/data_qap.xlsx
+++ b/TS_HW5/data_qap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cro0010\PycharmProjects\adaptive_optimization\Simulated_Annealing_HW1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\PycharmProjects\adaptive_optimization\TS_HW5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29E419E-C32E-49C9-AEE6-15488C109A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E287547D-B74C-4E2A-A802-24A40878DFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7ED01471-F3C8-4676-AF07-650F9DCA2BE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{7ED01471-F3C8-4676-AF07-650F9DCA2BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Distance" sheetId="1" r:id="rId1"/>
@@ -381,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E113B75-BBA8-427A-A222-5717794ABFDF}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -435,8 +435,23 @@
       <c r="O1">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1">
+        <v>3</v>
+      </c>
+      <c r="Q1">
+        <v>4</v>
+      </c>
+      <c r="R1">
+        <v>5</v>
+      </c>
+      <c r="S1">
+        <v>6</v>
+      </c>
+      <c r="T1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -482,8 +497,23 @@
       <c r="O2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2">
+        <v>3</v>
+      </c>
+      <c r="R2">
+        <v>4</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -529,8 +559,23 @@
       <c r="O3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>4</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -576,8 +621,23 @@
       <c r="O4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -623,8 +683,23 @@
       <c r="O5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -670,8 +745,23 @@
       <c r="O6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
+      <c r="T6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -717,8 +807,23 @@
       <c r="O7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -764,8 +869,23 @@
       <c r="O8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+      <c r="T8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -811,8 +931,23 @@
       <c r="O9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9">
+        <v>3</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -858,8 +993,23 @@
       <c r="O10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>3</v>
+      </c>
+      <c r="T10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -905,8 +1055,23 @@
       <c r="O11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <v>4</v>
+      </c>
+      <c r="T11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -952,8 +1117,23 @@
       <c r="O12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>3</v>
+      </c>
+      <c r="T12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -999,8 +1179,23 @@
       <c r="O13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>2</v>
+      </c>
+      <c r="T13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1046,8 +1241,23 @@
       <c r="O14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1091,6 +1301,331 @@
         <v>1</v>
       </c>
       <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15">
+        <v>4</v>
+      </c>
+      <c r="R15">
+        <v>3</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
+      </c>
+      <c r="T16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+      <c r="O17">
+        <v>4</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>3</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>4</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
         <v>0</v>
       </c>
     </row>
@@ -1102,132 +1637,162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FE1CF3-A94D-4010-ADE2-07A93FE2127B}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N1">
         <v>0</v>
       </c>
       <c r="O1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="P1">
+        <v>4</v>
+      </c>
+      <c r="Q1">
+        <v>4</v>
+      </c>
+      <c r="R1">
+        <v>0</v>
+      </c>
+      <c r="S1">
+        <v>0</v>
+      </c>
+      <c r="T1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>2</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K2">
         <v>2</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>5</v>
+      </c>
+      <c r="S2">
+        <v>10</v>
+      </c>
+      <c r="T2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -1236,30 +1801,45 @@
         <v>5</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>5</v>
       </c>
       <c r="O3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1268,45 +1848,60 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>5</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M4">
         <v>2</v>
       </c>
       <c r="N4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1315,57 +1910,72 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H5">
         <v>5</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -1374,7 +1984,7 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1383,21 +1993,36 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1406,412 +2031,857 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>10</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
         <v>6</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>5</v>
-      </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>5</v>
+      </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>5</v>
+      </c>
+      <c r="S15">
+        <v>10</v>
+      </c>
+      <c r="T15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>10</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>5</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>5</v>
+      </c>
+      <c r="S17">
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+      <c r="O18">
+        <v>5</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>5</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>5</v>
+      </c>
+      <c r="O19">
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
         <v>6</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>5</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>10</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>5</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>10</v>
-      </c>
-      <c r="L9">
-        <v>5</v>
-      </c>
-      <c r="M9">
-        <v>10</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>4</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>10</v>
-      </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>5</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>5</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>5</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12">
-        <v>5</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>3</v>
-      </c>
-      <c r="N12">
-        <v>3</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-      <c r="I13">
-        <v>10</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>3</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>10</v>
-      </c>
-      <c r="O13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>5</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>5</v>
-      </c>
-      <c r="L14">
-        <v>3</v>
-      </c>
-      <c r="M14">
-        <v>10</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>10</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>5</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
-      <c r="N15">
-        <v>4</v>
-      </c>
-      <c r="O15">
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>10</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>6</v>
+      </c>
+      <c r="T20">
         <v>0</v>
       </c>
     </row>

</xml_diff>